<commit_message>
config mapping with crud in frontend
</commit_message>
<xml_diff>
--- a/SmartDietAPI/Data/dishes.xlsx
+++ b/SmartDietAPI/Data/dishes.xlsx
@@ -5,25 +5,25 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FFF\Sem_8\EXE\SmartDietAPI\SmartDietAPI\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FFF\Sem_8\EXE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A56BAC7-1014-4355-A6E0-6592B01EFBAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4346C3B2-C85B-4E2D-A618-257618DDAAC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="16990" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10050" yWindow="1710" windowWidth="16990" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Món ăn" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Món ăn'!$A$1:$K$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Món ăn'!$A$1:$K$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>Tên món ăn</t>
   </si>
@@ -56,13 +56,105 @@
   </si>
   <si>
     <t>Feedback</t>
+  </si>
+  <si>
+    <t>Ba rọi rim cháy cạnh</t>
+  </si>
+  <si>
+    <t>Nam</t>
+  </si>
+  <si>
+    <t>Giàu protein</t>
+  </si>
+  <si>
+    <t>Ba rọi rim cháy cạnh ngon bắt cơm với nước rim khô kẹo, miếng thịt cháy cạnh rám mặt mềm bên trong.
+Có màu caramel đặc trưng của các món kho
+Dậy mùi kho đặc trưng của món Việt</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Link công thức - Google Tài liệu</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Ba rọi rim cháy cạnh | Món Ngon Mỗi Ngày</t>
+    </r>
+  </si>
+  <si>
+    <t>Chờ kiểm tra</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>M134-M204 - Google Drive</t>
+    </r>
+  </si>
+  <si>
+    <t>Huỳnh Nhật</t>
+  </si>
+  <si>
+    <t>Bạch Tuộc Ngâm Sả Tắc Chua Cay</t>
+  </si>
+  <si>
+    <t>Chung</t>
+  </si>
+  <si>
+    <t>Giàu calo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Từng con bạch tuộc sau khi hấp xong mềm, dai dai, không có vị tanh nhờ có gừng. Sả, tắc, ớt kết hợp làm cho món ăn trở nên đẹp mắt, thu hút.</t>
+  </si>
+  <si>
+    <t>Chi_thông tin món ăn</t>
+  </si>
+  <si>
+    <t>https://www.cooky.vn/cong-thuc/bach-tuoc-ngam-sa-tac-chua-cay-18935</t>
+  </si>
+  <si>
+    <t>M104.jpeg</t>
+  </si>
+  <si>
+    <t>Linh Chi</t>
+  </si>
+  <si>
+    <t>Bánh bao súp - Xiao long bao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cách làm bánh bao hấp đơn giản với lớp vỏ bánh dai mỏng bên ngoài, bao bọc nhân thịt, nước súp chảy ra từ bên trong bánh rất đặc trưng và hấp dẫn. </t>
+  </si>
+  <si>
+    <t>https://www.cooky.vn/cong-thuc/banh-bao-sup-xiao-long-bao-34747</t>
+  </si>
+  <si>
+    <t>M113.jpeg</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -85,20 +177,108 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FFFFCFC9"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF005A55"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF111111"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0A53A8"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6F8F9"/>
+        <bgColor rgb="FFF6F8F9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -148,6 +328,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF292F50"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF292F50"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
       </bottom>
       <diagonal/>
     </border>
@@ -196,11 +391,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF6F8F9"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFF6F8F9"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF6F8F9"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFF6F8F9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF6F8F9"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF292F50"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF6F8F9"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFF6F8F9"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -221,22 +446,88 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -317,8 +608,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Meal_Data" displayName="Meal_Data" ref="A1:K2" insertRow="1">
-  <autoFilter ref="A1:K2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Meal_Data" displayName="Meal_Data" ref="A1:K7">
+  <autoFilter ref="A1:K7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Tên món ăn"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Vùng miền"/>
@@ -537,13 +828,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z2"/>
+  <dimension ref="A1:Z7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -609,41 +900,196 @@
       <c r="Y1" s="7"/>
       <c r="Z1" s="7"/>
     </row>
-    <row r="2" spans="1:26" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="10"/>
+    <row r="2" spans="1:26" ht="93" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="12"/>
+      <c r="F2" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="15"/>
+    </row>
+    <row r="3" spans="1:26" ht="62" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="20"/>
+      <c r="F3" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="25"/>
+    </row>
+    <row r="4" spans="1:26" ht="62" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="12"/>
+      <c r="F4" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="15"/>
+    </row>
+    <row r="5" spans="1:26" ht="62" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="15"/>
+    </row>
+    <row r="6" spans="1:26" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="25"/>
+    </row>
+    <row r="7" spans="1:26" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="15"/>
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" sqref="J2" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="J2:J7" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Huỳnh Nhật,Linh Chi,Anh Khoa"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="E2" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" sqref="E2:E7" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Option 1,Option 2"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B2" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" sqref="B2:B7" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Bắc,Trung,Nam,Chung"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="H2" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" sqref="H2:H7" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"Chờ kiểm tra,Đợi Feedback,Đã Feedback,Đã xong"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showDropDown="1" sqref="A2 K2 I2 F2:G2 D2" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation type="list" allowBlank="1" sqref="C2" xr:uid="{00000000-0002-0000-0000-000006000000}">
+    <dataValidation allowBlank="1" showDropDown="1" sqref="A2:A7 D2:D7 F2:G7 I2:I7 K2:K7" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation type="list" allowBlank="1" sqref="C2:C7" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>"Không,Lỏng,Ít calo,Giàu calo,Ít cholesterol,Ăn chay,Ít natri,Giàu protein,Ít protein"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="I2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G3" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="I3" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F4" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G4" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="I4" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F5" r:id="rId10" xr:uid="{E83144F5-0C45-451B-A34F-052F0F0C44E3}"/>
+    <hyperlink ref="G5" r:id="rId11" xr:uid="{D032FBAE-3DB7-4E2C-A7CD-95C6D4A798E3}"/>
+    <hyperlink ref="I5" r:id="rId12" xr:uid="{4282001B-9FB0-45EF-9E07-0F0CBE2362DE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId13"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>